<commit_message>
added files from siemens laptop
</commit_message>
<xml_diff>
--- a/Stundenaufzeichnung.xlsx
+++ b/Stundenaufzeichnung.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -63,11 +63,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h&quot;h&quot;\ mm&quot;min&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,19 +307,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17"/>
-    <cellStyle name="Überschrift 4" xfId="4" builtinId="19"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17"/>
+    <cellStyle name="Heading 4" xfId="4" builtinId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -377,7 +377,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -412,7 +412,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -589,21 +589,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
@@ -616,21 +616,21 @@
     <col min="17" max="17" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="61.5" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:5" ht="61.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:5" ht="20.25" thickBot="1">
+      <c r="A3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickTop="1">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -639,17 +639,17 @@
         <v>0.21874999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2"/>
       <c r="B5" s="12"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="18" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -658,7 +658,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="A10" s="8" t="s">
         <v>3</v>
       </c>
@@ -675,11 +675,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.75" thickTop="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="10" t="str">
@@ -687,11 +687,11 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="5"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="10" t="str">
@@ -699,17 +699,17 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="13">
         <v>42803</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="21">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="21">
         <v>0.64583333333333337</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="10">
@@ -717,17 +717,17 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="13">
         <v>42811</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="21">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="21">
         <v>0.625</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="20" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="10">
@@ -735,9 +735,9 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="30">
       <c r="A15" s="13">
-        <v>42771</v>
+        <v>42992</v>
       </c>
       <c r="B15" s="14">
         <v>0.38541666666666669</v>
@@ -753,49 +753,49 @@
         <v>0.11458333333333331</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="13"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="17"/>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="18"/>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="13"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="18"/>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="13"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="18"/>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="13"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="18"/>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="13"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="18"/>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="5"/>
       <c r="D22" s="18"/>
       <c r="E22" s="10" t="str">
@@ -803,7 +803,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="5"/>
       <c r="D23" s="18"/>
       <c r="E23" s="10" t="str">
@@ -811,7 +811,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="5"/>
       <c r="D24" s="18"/>
       <c r="E24" s="10" t="str">
@@ -819,7 +819,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="5"/>
       <c r="D25" s="18"/>
       <c r="E25" s="10" t="str">
@@ -827,7 +827,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="5"/>
       <c r="D26" s="18"/>
       <c r="E26" s="10" t="str">
@@ -835,7 +835,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="5"/>
       <c r="D27" s="18"/>
       <c r="E27" s="10" t="str">
@@ -843,7 +843,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="5"/>
       <c r="D28" s="18"/>
       <c r="E28" s="10" t="str">
@@ -851,7 +851,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="5"/>
       <c r="D29" s="18"/>
       <c r="E29" s="10" t="str">
@@ -859,7 +859,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="5"/>
       <c r="D30" s="18"/>
       <c r="E30" s="10" t="str">
@@ -867,7 +867,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="5"/>
       <c r="D31" s="18"/>
       <c r="E31" s="10" t="str">
@@ -875,7 +875,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="5"/>
       <c r="D32" s="18"/>
       <c r="E32" s="10" t="str">
@@ -883,7 +883,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="5"/>
       <c r="D33" s="18"/>
       <c r="E33" s="10" t="str">
@@ -891,7 +891,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="5"/>
       <c r="D34" s="18"/>
       <c r="E34" s="10" t="str">
@@ -899,7 +899,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="5"/>
       <c r="D35" s="18"/>
       <c r="E35" s="10" t="str">
@@ -907,7 +907,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="15.75" thickBot="1">
       <c r="A36" s="5"/>
       <c r="D36" s="18"/>
       <c r="E36" s="10" t="str">
@@ -915,7 +915,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15.75" thickTop="1">
       <c r="A37" s="6"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>

</xml_diff>